<commit_message>
Incluido índice de Besson (Lluvioso) e índice de irregularidad temporal.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Enriquito\Trabajos e Investigaciones\Doctorado UNICA\Code\Pruebas\Get Rainy Streak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Enriquito\Trabajos e Investigaciones\Doctorado UNICA\Code\Pruebas\rainy_streak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15255C5-30DD-46FB-BCAE-5668CB68671A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EC1CE3-6DCB-4756-880E-0E6440D1008D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Promedio de días lluvuiosos</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Promedio de días lluviosos</t>
   </si>
   <si>
     <t>Cantidad promedio de rachas</t>
   </si>
   <si>
-    <t>Duración media de las rachas</t>
+    <t>Cantidad promedio de rachas de más de un día</t>
+  </si>
+  <si>
+    <t>Duración media de las rachas (Todas)</t>
+  </si>
+  <si>
+    <t>Probabilidad media de días lluviosos</t>
+  </si>
+  <si>
+    <t>Probabilidad media de días lluviosos si llovió el anterior</t>
+  </si>
+  <si>
+    <t>Coeficiente de Besson</t>
+  </si>
+  <si>
+    <t>Índice de irregularidad temporal</t>
   </si>
   <si>
     <t>mes 1</t>
@@ -71,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +96,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,17 +142,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -466,197 +498,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5">
         <v>3.8735955056179781</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>2.72752808988764</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
+        <v>0.7837078651685393</v>
+      </c>
+      <c r="E2" s="5">
         <v>1.433393525949705</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="4">
+        <v>0.1249377038782169</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.21672209656760219</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.1114194470611314</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.26219601584003538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5">
         <v>3.2732394366197179</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>2.3718309859154929</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
+        <v>0.6507042253521127</v>
+      </c>
+      <c r="E3" s="5">
         <v>1.423534540576793</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="4">
+        <v>0.1159268253197346</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.2030538788285268</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.1040258428453498</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.26080985673628843</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5">
         <v>3.579387186629527</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>2.6796657381615598</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
+        <v>0.62395543175487467</v>
+      </c>
+      <c r="E4" s="5">
         <v>1.296153335986205</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="4">
+        <v>0.11545848683619379</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.1609563602599815</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5.8258614714612862E-2</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.27998156310202882</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5">
         <v>3.878378378378379</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>2.6918918918918919</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
+        <v>0.74864864864864866</v>
+      </c>
+      <c r="E5" s="5">
         <v>1.449430501930502</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="4">
+        <v>0.12926765475152599</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.2222877422877424</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.11436898014038389</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.33995218365974028</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5">
         <v>8.3292682926829276</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>3.9317073170731711</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
+        <v>1.9146341463414629</v>
+      </c>
+      <c r="E6" s="5">
         <v>2.3917392566782811</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="4">
+        <v>0.26866148701809561</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.46059140323544118</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.27413728988992159</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.76420218783685578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5">
         <v>9.7362110311750598</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>5.0119904076738608</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
+        <v>2.167865707434053</v>
+      </c>
+      <c r="E7" s="5">
         <v>1.9863604354611559</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="4">
+        <v>0.32451716046517642</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.41498451421228832</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.14224061283339651</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.94506850633060169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5">
         <v>7.3607748184019366</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>4.7990314769975786</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
+        <v>1.554479418886199</v>
+      </c>
+      <c r="E8" s="5">
         <v>1.5243062761827879</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="4">
+        <v>0.2374297039756309</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.27954130429383262</v>
+      </c>
+      <c r="H8" s="5">
+        <v>6.0735439119462713E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.6320988037655606</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
         <v>9.3100961538461533</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>5.2427884615384617</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
+        <v>2.1490384615384621</v>
+      </c>
+      <c r="E9" s="5">
         <v>1.7979129377566869</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="4">
+        <v>0.30032196675971912</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.37149677060993369</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.1089652582711768</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.7859253995556954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
         <v>10.39182692307692</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>5.5192307692307692</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
+        <v>2.504807692307693</v>
+      </c>
+      <c r="E10" s="5">
         <v>1.905678609584861</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="4">
+        <v>0.34639565685519541</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.41132927609497538</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.1037483005218994</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.9416550972530815</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5">
         <v>9.3381294964028783</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>4.9232613908872898</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
+        <v>1.9928057553956831</v>
+      </c>
+      <c r="E11" s="5">
         <v>1.97521316280309</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="4">
+        <v>0.3012111278718963</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.39657771763109212</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.14854759191631159</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.80626652123412956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="B12" s="5">
         <v>6.14</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>3.3875000000000002</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
+        <v>1.2424999999999999</v>
+      </c>
+      <c r="E12" s="5">
         <v>1.857192460317461</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="4">
+        <v>0.2046639784946237</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.3381940749846129</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.18109996176665821</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.48407981080511819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5">
         <v>4.2022792022792022</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>2.8148148148148149</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
+        <v>0.81481481481481477</v>
+      </c>
+      <c r="E13" s="5">
         <v>1.4343033509700169</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.13555739362190969</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.2044166645109991</v>
+      </c>
+      <c r="H13" s="5">
+        <v>8.9812872105891339E-2</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.28141457297832201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incluido en el código la duración de las rachas de más de un día.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Enriquito\Trabajos e Investigaciones\Doctorado UNICA\Code\Pruebas\rainy_streak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EC1CE3-6DCB-4756-880E-0E6440D1008D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7044E7DF-0B31-464D-B05B-D40A018B3977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Promedio de días lluviosos</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Cantidad promedio de rachas de más de un día</t>
+  </si>
+  <si>
+    <t>Duración media de las rachas de más de un día</t>
   </si>
   <si>
     <t>Duración media de las rachas (Todas)</t>
@@ -86,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,13 +99,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -142,27 +138,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -498,388 +484,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>3.8735955056179781</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2">
         <v>2.72752808988764</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2">
         <v>0.7837078651685393</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
+        <v>2.4340206185567008</v>
+      </c>
+      <c r="F2">
         <v>1.433393525949705</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2">
         <v>0.1249377038782169</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2">
         <v>0.21672209656760219</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2">
         <v>0.1114194470611314</v>
       </c>
-      <c r="I2" s="5">
+      <c r="J2">
         <v>0.26219601584003538</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>3.2732394366197179</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>2.3718309859154929</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>0.6507042253521127</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
+        <v>2.3906810035842301</v>
+      </c>
+      <c r="F3">
         <v>1.423534540576793</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3">
         <v>0.1159268253197346</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3">
         <v>0.2030538788285268</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3">
         <v>0.1040258428453498</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3">
         <v>0.26080985673628843</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5">
+        <v>11</v>
+      </c>
+      <c r="B4">
         <v>3.579387186629527</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
         <v>2.6796657381615598</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>0.62395543175487467</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
+        <v>2.4291938997821352</v>
+      </c>
+      <c r="F4">
         <v>1.296153335986205</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4">
         <v>0.11545848683619379</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4">
         <v>0.1609563602599815</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4">
         <v>5.8258614714612862E-2</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4">
         <v>0.27998156310202882</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="5">
+        <v>12</v>
+      </c>
+      <c r="B5">
         <v>3.878378378378379</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5">
         <v>2.6918918918918919</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>0.74864864864864866</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
+        <v>2.6268472906403941</v>
+      </c>
+      <c r="F5">
         <v>1.449430501930502</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5">
         <v>0.12926765475152599</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5">
         <v>0.2222877422877424</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5">
         <v>0.11436898014038389</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5">
         <v>0.33995218365974028</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5">
+        <v>13</v>
+      </c>
+      <c r="B6">
         <v>8.3292682926829276</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6">
         <v>3.9317073170731711</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>1.9146341463414629</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
+        <v>3.4889037433155088</v>
+      </c>
+      <c r="F6">
         <v>2.3917392566782811</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6">
         <v>0.26866148701809561</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6">
         <v>0.46059140323544118</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6">
         <v>0.27413728988992159</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6">
         <v>0.76420218783685578</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5">
+        <v>14</v>
+      </c>
+      <c r="B7">
         <v>9.7362110311750598</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7">
         <v>5.0119904076738608</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7">
         <v>2.167865707434053</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7">
+        <v>3.2087365591397838</v>
+      </c>
+      <c r="F7">
         <v>1.9863604354611559</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7">
         <v>0.32451716046517642</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7">
         <v>0.41498451421228832</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7">
         <v>0.14224061283339651</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7">
         <v>0.94506850633060169</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5">
+        <v>15</v>
+      </c>
+      <c r="B8">
         <v>7.3607748184019366</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8">
         <v>4.7990314769975786</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <v>1.554479418886199</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
+        <v>2.6650326797385619</v>
+      </c>
+      <c r="F8">
         <v>1.5243062761827879</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8">
         <v>0.2374297039756309</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8">
         <v>0.27954130429383262</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8">
         <v>6.0735439119462713E-2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8">
         <v>0.6320988037655606</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5">
+        <v>16</v>
+      </c>
+      <c r="B9">
         <v>9.3100961538461533</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9">
         <v>5.2427884615384617</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <v>2.1490384615384621</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9">
+        <v>2.8909722222222221</v>
+      </c>
+      <c r="F9">
         <v>1.7979129377566869</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9">
         <v>0.30032196675971912</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9">
         <v>0.37149677060993369</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9">
         <v>0.1089652582711768</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9">
         <v>0.7859253995556954</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5">
+        <v>17</v>
+      </c>
+      <c r="B10">
         <v>10.39182692307692</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10">
         <v>5.5192307692307692</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <v>2.504807692307693</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10">
+        <v>2.9120974760661449</v>
+      </c>
+      <c r="F10">
         <v>1.905678609584861</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10">
         <v>0.34639565685519541</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10">
         <v>0.41132927609497538</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10">
         <v>0.1037483005218994</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10">
         <v>0.9416550972530815</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5">
+        <v>18</v>
+      </c>
+      <c r="B11">
         <v>9.3381294964028783</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11">
         <v>4.9232613908872898</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <v>1.9928057553956831</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11">
+        <v>3.2878240740740741</v>
+      </c>
+      <c r="F11">
         <v>1.97521316280309</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11">
         <v>0.3012111278718963</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11">
         <v>0.39657771763109212</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11">
         <v>0.14854759191631159</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11">
         <v>0.80626652123412956</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="5">
+        <v>19</v>
+      </c>
+      <c r="B12">
         <v>6.14</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12">
         <v>3.3875000000000002</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12">
         <v>1.2424999999999999</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12">
+        <v>3.2688552188552191</v>
+      </c>
+      <c r="F12">
         <v>1.857192460317461</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12">
         <v>0.2046639784946237</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12">
         <v>0.3381940749846129</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12">
         <v>0.18109996176665821</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12">
         <v>0.48407981080511819</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="5">
+        <v>20</v>
+      </c>
+      <c r="B13">
         <v>4.2022792022792022</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13">
         <v>2.8148148148148149</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <v>0.81481481481481477</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13">
+        <v>2.5758003766478339</v>
+      </c>
+      <c r="F13">
         <v>1.4343033509700169</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13">
         <v>0.13555739362190969</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13">
         <v>0.2044166645109991</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13">
         <v>8.9812872105891339E-2</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13">
         <v>0.28141457297832201</v>
       </c>
     </row>

</xml_diff>